<commit_message>
Book a class Commit
</commit_message>
<xml_diff>
--- a/TestDataXls/student_book_a_class.xlsx
+++ b/TestDataXls/student_book_a_class.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="class_booking" sheetId="1" r:id="rId2"/>
-    <sheet name="stu" sheetId="3" r:id="rId3"/>
+    <sheet name="class_booking" sheetId="1" r:id="rId1"/>
+    <sheet name="stu" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,8 +24,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="J2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+0 - Session
+1 - Subscription
+2 - Monthly</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="152">
   <si>
     <t>password</t>
   </si>
@@ -470,6 +505,18 @@
   </si>
   <si>
     <t>12/25</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>sendhan-therapist/personal-growth-online-grp-pre-scho-begi-thurs</t>
+  </si>
+  <si>
+    <t>sen2023</t>
+  </si>
+  <si>
+    <t>Thursday</t>
   </si>
 </sst>
 </file>
@@ -480,7 +527,7 @@
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +573,19 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -640,333 +700,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr lang="en-IN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>class_booking!$AI$1:$AI$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>expectedError</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Login Success &gt; Class booked</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Login Success &gt; Class booked</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Login Success &gt; Class booked</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>class_booking!#REF!</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F1F7-48B7-AD55-62773C69434F}"/>
-            </c:ext>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>class_booking!#REF!</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>#REF!</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="233791880"/>
-        <c:axId val="233792664"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="233791880"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-IN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="233792664"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="233792664"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-IN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="233791880"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8652387" cy="6276258"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1255,12 +988,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF6" sqref="AF6"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1019,7 @@
     <col min="21" max="21" width="12" customWidth="1"/>
     <col min="22" max="22" width="12.140625" style="12" customWidth="1"/>
     <col min="23" max="23" width="9.85546875" style="9" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" style="27" customWidth="1"/>
+    <col min="24" max="24" width="21.7109375" style="27" customWidth="1"/>
     <col min="25" max="25" width="13.28515625" customWidth="1"/>
     <col min="26" max="26" width="14.140625" style="16" customWidth="1"/>
     <col min="27" max="27" width="13.28515625" style="16" customWidth="1"/>
@@ -1413,7 +1146,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>17</v>
@@ -1425,22 +1158,22 @@
         <v>36</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
       <c r="I2" s="5">
         <v>2</v>
       </c>
       <c r="J2" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="L2" s="5">
         <v>0</v>
@@ -1449,20 +1182,20 @@
         <v>1</v>
       </c>
       <c r="N2" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O2" s="11">
         <f t="shared" ref="O2:O6" si="0">N2+R2</f>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="P2" s="8">
         <f t="shared" ref="P2:P37" si="1">(((M2+1)*O2)*I2)</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="11">
         <f t="shared" ref="R2:R6" si="2">N2*S2</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="S2" s="3">
         <v>0.25</v>
@@ -1472,15 +1205,15 @@
       </c>
       <c r="U2" s="6">
         <f t="shared" ref="U2:U6" si="3">P2*T2</f>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="V2" s="11">
         <f t="shared" ref="V2:V6" si="4">T2*P2</f>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="W2" s="8">
         <f t="shared" ref="W2:W6" si="5">P2+V2</f>
-        <v>40.4</v>
+        <v>50.5</v>
       </c>
       <c r="X2" s="20"/>
       <c r="Y2" s="3" t="s">
@@ -1491,19 +1224,19 @@
       </c>
       <c r="AA2" s="13">
         <f t="shared" ref="AA2:AA4" si="6">SUM(T2*AB2)</f>
-        <v>0.38</v>
+        <v>0.48</v>
       </c>
       <c r="AB2" s="9">
         <f t="shared" ref="AB2:AB4" si="7">SUM(P2-Z2)</f>
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="AC2" s="9">
         <f t="shared" ref="AC2:AC4" si="8">SUM(T2*AB2)</f>
-        <v>0.38</v>
+        <v>0.48</v>
       </c>
       <c r="AD2" s="9">
         <f t="shared" ref="AD2:AD4" si="9">SUM(AA2+AB2)</f>
-        <v>38.380000000000003</v>
+        <v>48.48</v>
       </c>
       <c r="AE2" s="4" t="s">
         <v>18</v>
@@ -1759,7 +1492,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>17</v>
@@ -11393,6 +11126,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId59"/>
+  <legacyDrawing r:id="rId60"/>
 </worksheet>
 </file>
 

</xml_diff>